<commit_message>
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C768905
</commit_message>
<xml_diff>
--- a/PPIUK-ResearchDocDisplay/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-ResearchDocDisplay/src/test/resources/CobaltUsers.xlsx
@@ -1054,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G84" sqref="A81:G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,18 +2577,6 @@
       <c r="G80" s="10" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="9"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="9"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="9"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>